<commit_message>
Update CTN Editorial Board Notes and ToDo lists Jan 21 2018.xlsx
</commit_message>
<xml_diff>
--- a/CTN Editorial Board Notes and ToDo lists Jan 21 2018.xlsx
+++ b/CTN Editorial Board Notes and ToDo lists Jan 21 2018.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Conferences and papers\CTN\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28028"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14955" windowHeight="7515" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19280" windowHeight="14280" tabRatio="856" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="To Do List" sheetId="1" r:id="rId1"/>
@@ -20,8 +15,11 @@
     <sheet name="hot topic list" sheetId="5" r:id="rId6"/>
     <sheet name="sample author instructions" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -30,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="72">
   <si>
     <t>Action</t>
   </si>
@@ -305,16 +303,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -404,7 +402,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -439,7 +437,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -616,7 +614,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -630,15 +628,15 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="40.5703125" customWidth="1"/>
-    <col min="3" max="3" width="23.5703125" customWidth="1"/>
+    <col min="2" max="2" width="40.5" customWidth="1"/>
+    <col min="3" max="3" width="23.5" customWidth="1"/>
     <col min="4" max="4" width="50" customWidth="1"/>
-    <col min="5" max="5" width="38.42578125" customWidth="1"/>
+    <col min="5" max="5" width="38.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:5">
       <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
@@ -652,7 +650,7 @@
         <v>43466</v>
       </c>
     </row>
-    <row r="5" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:5" ht="28">
       <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
@@ -666,7 +664,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:5" ht="28">
       <c r="B6" s="2" t="s">
         <v>16</v>
       </c>
@@ -678,7 +676,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:5">
       <c r="B7" s="2" t="s">
         <v>8</v>
       </c>
@@ -689,7 +687,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:5">
       <c r="B8" s="2" t="s">
         <v>9</v>
       </c>
@@ -698,7 +696,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:5">
       <c r="B9" s="2" t="s">
         <v>12</v>
       </c>
@@ -707,7 +705,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:5">
       <c r="B10" s="2" t="s">
         <v>59</v>
       </c>
@@ -716,164 +714,169 @@
       </c>
       <c r="D10" s="2"/>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:5">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:5">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:5">
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:5">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:5">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:5">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:4">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:4">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:4">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:4">
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:4">
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:4">
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:4">
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:4">
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:4">
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:4">
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:4">
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:4">
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:4">
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:4">
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:4">
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:4">
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -885,13 +888,13 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="40.85546875" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" customWidth="1"/>
+    <col min="2" max="2" width="40.83203125" customWidth="1"/>
+    <col min="3" max="3" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3">
       <c r="B3" t="s">
         <v>5</v>
       </c>
@@ -899,7 +902,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3">
       <c r="B4" t="s">
         <v>24</v>
       </c>
@@ -907,7 +910,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3">
       <c r="B5" t="s">
         <v>7</v>
       </c>
@@ -915,7 +918,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:3">
       <c r="B6" t="s">
         <v>22</v>
       </c>
@@ -923,7 +926,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:3">
       <c r="B7" t="s">
         <v>21</v>
       </c>
@@ -933,6 +936,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -944,14 +952,14 @@
       <selection activeCell="B4" sqref="B4:D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="38.7109375" customWidth="1"/>
-    <col min="3" max="3" width="34.28515625" customWidth="1"/>
-    <col min="4" max="4" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.6640625" customWidth="1"/>
+    <col min="3" max="3" width="34.33203125" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4">
       <c r="B3" t="s">
         <v>17</v>
       </c>
@@ -962,7 +970,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4">
       <c r="B4" t="s">
         <v>62</v>
       </c>
@@ -973,7 +981,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4">
       <c r="B5" t="s">
         <v>65</v>
       </c>
@@ -983,6 +991,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -994,28 +1007,33 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="128.42578125" customWidth="1"/>
+    <col min="2" max="2" width="128.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:2">
       <c r="B2" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="2:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:2" ht="42">
       <c r="B3" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="2:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:2" ht="28">
       <c r="B4" s="1" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1027,9 +1045,14 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1037,19 +1060,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" customWidth="1"/>
+    <col min="1" max="1" width="13.5" customWidth="1"/>
     <col min="2" max="2" width="63" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" customWidth="1"/>
+    <col min="3" max="3" width="16.5" customWidth="1"/>
     <col min="4" max="4" width="58" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="42">
       <c r="A1" s="5" t="s">
         <v>43</v>
       </c>
@@ -1058,17 +1081,17 @@
       </c>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="B3" s="2"/>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="42">
       <c r="A5" s="6" t="s">
         <v>45</v>
       </c>
@@ -1082,7 +1105,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="8" t="s">
         <v>26</v>
       </c>
@@ -1096,7 +1119,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="8"/>
       <c r="B7" s="8" t="s">
         <v>29</v>
@@ -1108,15 +1131,17 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="8"/>
       <c r="B8" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="9"/>
+      <c r="C8" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="D8" s="8"/>
     </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="28">
       <c r="A9" s="8"/>
       <c r="B9" s="8" t="s">
         <v>31</v>
@@ -1126,7 +1151,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="8"/>
       <c r="B10" s="8" t="s">
         <v>32</v>
@@ -1134,7 +1159,7 @@
       <c r="C10" s="9"/>
       <c r="D10" s="8"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" s="8"/>
       <c r="B11" s="8" t="s">
         <v>33</v>
@@ -1143,7 +1168,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="42">
       <c r="A12" s="8"/>
       <c r="B12" s="8" t="s">
         <v>35</v>
@@ -1155,7 +1180,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" s="8"/>
       <c r="B13" s="8" t="s">
         <v>36</v>
@@ -1167,7 +1192,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" s="8"/>
       <c r="B14" s="8" t="s">
         <v>37</v>
@@ -1175,7 +1200,7 @@
       <c r="C14" s="9"/>
       <c r="D14" s="8"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" s="8"/>
       <c r="B15" s="8" t="s">
         <v>38</v>
@@ -1185,7 +1210,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" s="8"/>
       <c r="B16" s="8" t="s">
         <v>69</v>
@@ -1195,7 +1220,7 @@
       </c>
       <c r="D16" s="8"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17" s="8"/>
       <c r="B17" s="8" t="s">
         <v>39</v>
@@ -1205,7 +1230,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18" s="8"/>
       <c r="B18" s="8" t="s">
         <v>52</v>
@@ -1215,7 +1240,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19" s="8"/>
       <c r="B19" s="8" t="s">
         <v>70</v>
@@ -1227,25 +1252,25 @@
         <v>71</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="A20" s="8"/>
       <c r="B20" s="8"/>
       <c r="C20" s="9"/>
       <c r="D20" s="8"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="A21" s="8"/>
       <c r="B21" s="8"/>
       <c r="C21" s="9"/>
       <c r="D21" s="8"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="A22" s="8"/>
       <c r="B22" s="8"/>
       <c r="C22" s="9"/>
       <c r="D22" s="8"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="A23" s="8"/>
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
@@ -1253,7 +1278,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1261,27 +1291,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="146.42578125" customWidth="1"/>
+    <col min="1" max="1" width="146.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:1" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" ht="56">
       <c r="A2" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" ht="28">
       <c r="A3" s="1" t="s">
         <v>41</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>